<commit_message>
updated infection R and template Excel
</commit_message>
<xml_diff>
--- a/Infection_data_template.xlsx
+++ b/Infection_data_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JQ/Documents/_CODE REPOS/GitHub/Survival_functions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD686609-0657-2C4E-B759-148E2FBCDF27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D81FF18-3EB1-F942-8C7B-4849C4C433F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11480" yWindow="460" windowWidth="36460" windowHeight="28340" activeTab="3" xr2:uid="{FF948C06-BD39-497C-ADCD-B8D8DC22913A}"/>
+    <workbookView xWindow="11480" yWindow="460" windowWidth="36460" windowHeight="28340" xr2:uid="{FF948C06-BD39-497C-ADCD-B8D8DC22913A}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="58">
   <si>
     <t>Date</t>
   </si>
@@ -436,6 +436,9 @@
 This is essential to perform the statistics right, to know the number of censored (still alive) flies at the end of the observational period.
 20 is (currently) the default value.</t>
     </r>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -1895,8 +1898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB3EAAA9-B59A-44C6-B69E-B4E274BF5D86}">
   <dimension ref="A1:J1117"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -15703,6 +15706,18 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{47F1B97B-C63B-B342-9C72-5F807C9D610E}">
+          <x14:formula1>
+            <xm:f>dropdown!B1:B3</xm:f>
+          </x14:formula1>
+          <xm:sqref>I2:I1117</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -15711,7 +15726,7 @@
   <dimension ref="A1:O234"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -19767,22 +19782,33 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0596E2C7-6F61-1E40-9697-BC06A07B8BB6}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2">
       <c r="A1" s="23" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="B1" s="23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" s="23" t="s">
         <v>55</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="B3" s="23" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -19794,7 +19820,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86A88E23-9106-8241-AB2A-7EBE0B3E0A8A}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update infection.R to make analyse_spreadsheet more modular; data template tweaked to match better
</commit_message>
<xml_diff>
--- a/Infection_data_template.xlsx
+++ b/Infection_data_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JQ/Documents/_CODE REPOS/GitHub/Survival_functions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D81FF18-3EB1-F942-8C7B-4849C4C433F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D4B1CC-A888-FE45-AE4E-40B315E6A1F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11480" yWindow="460" windowWidth="36460" windowHeight="28340" xr2:uid="{FF948C06-BD39-497C-ADCD-B8D8DC22913A}"/>
+    <workbookView xWindow="11480" yWindow="460" windowWidth="36460" windowHeight="28340" activeTab="2" xr2:uid="{FF948C06-BD39-497C-ADCD-B8D8DC22913A}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -438,7 +438,7 @@
     </r>
   </si>
   <si>
-    <t>NA</t>
+    <t>mixed</t>
   </si>
 </sst>
 </file>
@@ -1898,7 +1898,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB3EAAA9-B59A-44C6-B69E-B4E274BF5D86}">
   <dimension ref="A1:J1117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
@@ -19784,8 +19784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0596E2C7-6F61-1E40-9697-BC06A07B8BB6}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>